<commit_message>
Updated BOM and fixed some labels
</commit_message>
<xml_diff>
--- a/schematic/AutoDischarger/AutoDischargerBOM.xlsx
+++ b/schematic/AutoDischarger/AutoDischargerBOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AutoDischarger\schematic\AutoDischarger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBCB0D44-489C-473E-BF2A-16198901FB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01890E73-175E-40A1-8F7D-5D13EE084848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutoDischarger" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Source:</t>
   </si>
@@ -58,15 +58,6 @@
     <t>10 uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C3, </t>
-  </si>
-  <si>
-    <t>100 nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4, C5, C6, </t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -82,9 +73,6 @@
     <t xml:space="preserve">IC1, </t>
   </si>
   <si>
-    <t>AP7375-50SA-7</t>
-  </si>
-  <si>
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
@@ -176,12 +164,21 @@
   </si>
   <si>
     <t>SamacSys_Parts:PTS647SK38SMTR2LFS</t>
+  </si>
+  <si>
+    <t>AP7375-50W5-7</t>
+  </si>
+  <si>
+    <t>SOT95P285X140-5N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3, C4, C5, C6, </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1017,18 +1014,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1103,13 +1100,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1117,16 +1114,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1137,178 +1134,164 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>23</v>
-      </c>
-      <c r="D13" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
         <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1">
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="1">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="1">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="1">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="1">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="1">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pullup to MCLR
</commit_message>
<xml_diff>
--- a/schematic/AutoDischarger/AutoDischargerBOM.xlsx
+++ b/schematic/AutoDischarger/AutoDischargerBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AutoDischarger\schematic\AutoDischarger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01890E73-175E-40A1-8F7D-5D13EE084848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278790EC-49D5-416A-A7C5-D09B9F0D6C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Source:</t>
   </si>
   <si>
-    <t>C:\Projects\AutoDischarger\schematic\AutoDischarger\AutoDischarger.kicad_sch</t>
-  </si>
-  <si>
     <t>Component Count:</t>
   </si>
   <si>
@@ -173,6 +170,15 @@
   </si>
   <si>
     <t xml:space="preserve">C3, C4, C5, C6, </t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>AutoDischarger</t>
   </si>
 </sst>
 </file>
@@ -661,12 +667,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1022,276 +1026,285 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="19.08984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="2">
-        <v>44886.935486111113</v>
+      <c r="B3" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
+      <c r="A5" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
       <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
+      <c r="A8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>50</v>
+      <c r="A9" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
+      <c r="A10" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
+      <c r="A11" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
+      <c r="A12" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
+      <c r="A13" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
+      <c r="A14" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B14" s="1">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="1">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="1">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="1">
-        <v>6</v>
-      </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
         <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>